<commit_message>
Tentativa de pushar as alterações
</commit_message>
<xml_diff>
--- a/data/dados_vendas_google.xlsx
+++ b/data/dados_vendas_google.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win\Code\Python_101\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win\Code\Projetos\Python_101\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DAF7B8-E5DA-4B5B-B6C7-3E09C0A81A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31101DD2-2002-4ADE-AB8A-F776A7C5481D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,10 +32,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Receita</t>
+    <t>date</t>
   </si>
   <si>
-    <t>Índice do dia</t>
+    <t>receita</t>
   </si>
 </sst>
 </file>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1636"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1601" workbookViewId="0">
-      <selection activeCell="P1628" sqref="P1628"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -410,10 +410,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>